<commit_message>
add scored criteria, update summary
</commit_message>
<xml_diff>
--- a/casus/criteria_totaalscore.xlsx
+++ b/casus/criteria_totaalscore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvandenbrink\Documents\github\disgeo-imsor\casus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A96857-1696-4502-B187-1027D5B8F1EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A47198B-9EA5-43FE-9148-5814C678466C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="1335" windowWidth="20730" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5400" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Criteria" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +261,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +289,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -333,15 +345,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -379,13 +392,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Goed" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Invoer" xfId="5" builtinId="20"/>
     <cellStyle name="Kop 1" xfId="1" builtinId="16"/>
     <cellStyle name="Neutraal" xfId="4" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="6" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -700,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,16 +768,16 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="10"/>
@@ -775,13 +792,13 @@
       <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="15" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="15" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -799,16 +816,16 @@
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="15" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="10"/>
@@ -826,13 +843,13 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="15" t="s">
         <v>43</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="15" t="s">
         <v>42</v>
       </c>
       <c r="H5" s="10"/>
@@ -856,7 +873,7 @@
       <c r="F6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H6" s="10"/>
@@ -877,7 +894,7 @@
       <c r="E7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="15" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -898,10 +915,10 @@
       <c r="D8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="15" t="s">
         <v>42</v>
       </c>
       <c r="G8" s="10" t="s">
@@ -919,16 +936,16 @@
       <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="15" t="s">
         <v>49</v>
       </c>
       <c r="H9" s="10"/>

</xml_diff>